<commit_message>
dependancy on full wpf toolkit
</commit_message>
<xml_diff>
--- a/Site data.xlsx
+++ b/Site data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Site Id No</t>
   </si>
@@ -27,9 +27,6 @@
     <t>medical record format</t>
   </si>
   <si>
-    <t>Pondicherry</t>
-  </si>
-  <si>
     <t>trial commencement date</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>Pondicherry -???</t>
   </si>
 </sst>
 </file>
@@ -384,27 +384,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -414,34 +417,37 @@
       <c r="C2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>